<commit_message>
[PATCH] Arreglo todas las queries hasta ahora :)
</commit_message>
<xml_diff>
--- a/Listado Articulos.xlsx
+++ b/Listado Articulos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="96">
   <si>
     <t>Marca</t>
   </si>
@@ -32,12 +32,48 @@
     <t>Bomba de aceite</t>
   </si>
   <si>
-    <t>CARESA6325</t>
+    <t>CARESA1275</t>
+  </si>
+  <si>
+    <t>Centrinel</t>
+  </si>
+  <si>
+    <t>Aros recambio</t>
+  </si>
+  <si>
+    <t>CNA7604</t>
+  </si>
+  <si>
+    <t>Aros rectificación</t>
+  </si>
+  <si>
+    <t>CMA7604</t>
+  </si>
+  <si>
+    <t>Co-ber</t>
+  </si>
+  <si>
+    <t>Pernos</t>
+  </si>
+  <si>
+    <t>N-1037A</t>
+  </si>
+  <si>
+    <t>N-1039</t>
+  </si>
+  <si>
+    <t>N-1040</t>
   </si>
   <si>
     <t>Garbossa</t>
   </si>
   <si>
+    <t>Bujes de biela</t>
+  </si>
+  <si>
+    <t>I-42</t>
+  </si>
+  <si>
     <t>Bujes de leva</t>
   </si>
   <si>
@@ -47,22 +83,61 @@
     <t>Illinois</t>
   </si>
   <si>
+    <t>Juego juntas descarb.</t>
+  </si>
+  <si>
+    <t>JD-174-ST</t>
+  </si>
+  <si>
+    <t>Juego de tornillos</t>
+  </si>
+  <si>
+    <t>BU-016</t>
+  </si>
+  <si>
+    <t>Junta tapa de cilindros</t>
+  </si>
+  <si>
+    <t>TC-628-20 1M</t>
+  </si>
+  <si>
     <t>Juego juntas</t>
   </si>
   <si>
-    <t>JR-333-15</t>
-  </si>
-  <si>
-    <t>Juego de tornillos</t>
-  </si>
-  <si>
-    <t>BU-052</t>
-  </si>
-  <si>
-    <t>Junta tapa de cilindros</t>
-  </si>
-  <si>
-    <t>TC-491-15</t>
+    <t>JR-340-15</t>
+  </si>
+  <si>
+    <t>BU-006</t>
+  </si>
+  <si>
+    <t>TC-534-15</t>
+  </si>
+  <si>
+    <t>JD-135-15</t>
+  </si>
+  <si>
+    <t>JR-358-15</t>
+  </si>
+  <si>
+    <t>TC-617-15</t>
+  </si>
+  <si>
+    <t>JD-295-15</t>
+  </si>
+  <si>
+    <t>JR-492-15</t>
+  </si>
+  <si>
+    <t>BU-009</t>
+  </si>
+  <si>
+    <t>TC-725-15</t>
+  </si>
+  <si>
+    <t>JD-492-15</t>
+  </si>
+  <si>
+    <t>JR-551-15</t>
   </si>
   <si>
     <t>Mai</t>
@@ -71,12 +146,27 @@
     <t>Kit de retenes</t>
   </si>
   <si>
-    <t>9490</t>
+    <t>9035</t>
+  </si>
+  <si>
+    <t>9562</t>
   </si>
   <si>
     <t>Nubo</t>
   </si>
   <si>
+    <t>Casquillos admisión</t>
+  </si>
+  <si>
+    <t>CF139</t>
+  </si>
+  <si>
+    <t>Casquillos escape</t>
+  </si>
+  <si>
+    <t>C140</t>
+  </si>
+  <si>
     <t>Válvulas admisión</t>
   </si>
   <si>
@@ -89,22 +179,70 @@
     <t>23345-ECB</t>
   </si>
   <si>
-    <t>3146-AC</t>
-  </si>
-  <si>
-    <t>3147-ECB</t>
+    <t>c237</t>
+  </si>
+  <si>
+    <t>C225</t>
+  </si>
+  <si>
+    <t>1175-EC</t>
+  </si>
+  <si>
+    <t>1826-AC</t>
+  </si>
+  <si>
+    <t>C269</t>
+  </si>
+  <si>
+    <t>C330</t>
+  </si>
+  <si>
+    <t>3800-AC</t>
+  </si>
+  <si>
+    <t>3801-EC</t>
+  </si>
+  <si>
+    <t>C311</t>
+  </si>
+  <si>
+    <t>3514-AC</t>
+  </si>
+  <si>
+    <t>3515-EC</t>
   </si>
   <si>
     <t>Power enginne</t>
   </si>
   <si>
+    <t>808316</t>
+  </si>
+  <si>
+    <t>818316</t>
+  </si>
+  <si>
     <t>Sub conjunto motor</t>
   </si>
   <si>
+    <t>62280</t>
+  </si>
+  <si>
+    <t>62084</t>
+  </si>
+  <si>
+    <t>817508</t>
+  </si>
+  <si>
+    <t>807508</t>
+  </si>
+  <si>
     <t>62580</t>
   </si>
   <si>
-    <t>62179</t>
+    <t>816083</t>
+  </si>
+  <si>
+    <t>62386</t>
   </si>
   <si>
     <t>Sgb</t>
@@ -113,19 +251,37 @@
     <t>Juego cojinetes de bancada</t>
   </si>
   <si>
+    <t>M383-5A</t>
+  </si>
+  <si>
+    <t>Juego cojinetes de biela</t>
+  </si>
+  <si>
+    <t>R383-4A</t>
+  </si>
+  <si>
+    <t>M385-5A</t>
+  </si>
+  <si>
+    <t>R395-4A</t>
+  </si>
+  <si>
+    <t>M377-5A</t>
+  </si>
+  <si>
+    <t>R372-4A</t>
+  </si>
+  <si>
     <t>M944-5A</t>
   </si>
   <si>
-    <t>Juego cojinetes de biela</t>
-  </si>
-  <si>
     <t>R944-4A</t>
   </si>
   <si>
-    <t>M222-5A</t>
-  </si>
-  <si>
-    <t>R223-4A</t>
+    <t>Ten-up</t>
+  </si>
+  <si>
+    <t>K166P</t>
   </si>
   <si>
     <t>Weskan</t>
@@ -134,7 +290,16 @@
     <t>Guías</t>
   </si>
   <si>
-    <t>1717B</t>
+    <t>1948</t>
+  </si>
+  <si>
+    <t>1593B</t>
+  </si>
+  <si>
+    <t>1593</t>
+  </si>
+  <si>
+    <t>1588B</t>
   </si>
 </sst>
 </file>
@@ -186,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -222,13 +387,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>1.0</v>
@@ -236,13 +401,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>1.0</v>
@@ -250,13 +415,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
         <v>1.0</v>
@@ -264,13 +429,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
         <v>1.0</v>
@@ -278,13 +443,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
         <v>1.0</v>
@@ -292,13 +457,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" t="n">
         <v>1.0</v>
@@ -306,13 +471,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
         <v>1.0</v>
@@ -320,13 +485,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
       </c>
       <c r="D10" t="n">
         <v>1.0</v>
@@ -334,13 +499,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="n">
         <v>1.0</v>
@@ -348,13 +513,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" t="n">
         <v>1.0</v>
@@ -362,13 +527,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
       </c>
       <c r="D13" t="n">
         <v>1.0</v>
@@ -376,13 +541,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14" t="n">
         <v>1.0</v>
@@ -390,41 +555,41 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
       <c r="D15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
       <c r="D16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D17" t="n">
         <v>1.0</v>
@@ -432,16 +597,688 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D23" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D24" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
         <v>40</v>
       </c>
-      <c r="D18" t="n">
-        <v>1.0</v>
+      <c r="D25" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" t="s">
+        <v>94</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" t="s">
+        <v>91</v>
+      </c>
+      <c r="C66" t="s">
+        <v>95</v>
+      </c>
+      <c r="D66" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged in add_side_by_side_repository (pull request #66)
[MINOR] Add Side by side repositories

* [MINOR] Add Side by side repositories
</commit_message>
<xml_diff>
--- a/Listado Articulos.xlsx
+++ b/Listado Articulos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="98">
   <si>
     <t>Marca</t>
   </si>
@@ -35,6 +35,9 @@
     <t>CARESA1275</t>
   </si>
   <si>
+    <t>CARESA6325</t>
+  </si>
+  <si>
     <t>Centrinel</t>
   </si>
   <si>
@@ -107,12 +110,12 @@
     <t>JR-340-15</t>
   </si>
   <si>
+    <t>TC-534-15</t>
+  </si>
+  <si>
     <t>BU-006</t>
   </si>
   <si>
-    <t>TC-534-15</t>
-  </si>
-  <si>
     <t>JD-135-15</t>
   </si>
   <si>
@@ -210,6 +213,9 @@
   </si>
   <si>
     <t>3515-EC</t>
+  </si>
+  <si>
+    <t>1104-EP 0.8</t>
   </si>
   <si>
     <t>Power enginne</t>
@@ -351,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -401,13 +407,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>1.0</v>
@@ -415,13 +421,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5" t="n">
         <v>1.0</v>
@@ -429,13 +435,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
       <c r="D6" t="n">
         <v>1.0</v>
@@ -443,10 +449,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -457,10 +463,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -471,13 +477,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
       <c r="D9" t="n">
         <v>1.0</v>
@@ -485,13 +491,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
       <c r="D10" t="n">
         <v>1.0</v>
@@ -499,13 +505,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
       </c>
       <c r="D11" t="n">
         <v>1.0</v>
@@ -513,13 +519,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
       </c>
       <c r="D12" t="n">
         <v>1.0</v>
@@ -527,13 +533,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
       </c>
       <c r="D13" t="n">
         <v>1.0</v>
@@ -541,13 +547,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
       </c>
       <c r="D14" t="n">
         <v>1.0</v>
@@ -555,24 +561,24 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
       </c>
       <c r="D15" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -583,24 +589,24 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -611,27 +617,27 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D19" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" t="n">
         <v>2.0</v>
@@ -639,24 +645,24 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
         <v>36</v>
       </c>
       <c r="D21" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
@@ -667,24 +673,24 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -695,24 +701,24 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>40</v>
       </c>
       <c r="D25" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -723,38 +729,38 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D27" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D28" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
@@ -765,13 +771,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
         <v>46</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" t="s">
-        <v>48</v>
       </c>
       <c r="D30" t="n">
         <v>1.0</v>
@@ -779,13 +785,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
         <v>49</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
       </c>
       <c r="D31" t="n">
         <v>1.0</v>
@@ -793,27 +799,27 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
         <v>51</v>
       </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
       <c r="D32" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
         <v>53</v>
-      </c>
-      <c r="C33" t="s">
-        <v>54</v>
       </c>
       <c r="D33" t="n">
         <v>2.0</v>
@@ -821,24 +827,24 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
         <v>55</v>
       </c>
       <c r="D34" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -849,10 +855,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -863,10 +869,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
         <v>58</v>
@@ -877,10 +883,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
         <v>59</v>
@@ -891,10 +897,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
         <v>60</v>
@@ -905,10 +911,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
@@ -919,10 +925,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
         <v>62</v>
@@ -933,10 +939,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>63</v>
@@ -947,10 +953,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
         <v>64</v>
@@ -961,10 +967,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
         <v>65</v>
@@ -975,13 +981,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" t="s">
         <v>66</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>67</v>
       </c>
       <c r="D45" t="n">
         <v>1.0</v>
@@ -989,13 +995,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D46" t="n">
         <v>1.0</v>
@@ -1003,13 +1009,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
         <v>69</v>
-      </c>
-      <c r="C47" t="s">
-        <v>70</v>
       </c>
       <c r="D47" t="n">
         <v>1.0</v>
@@ -1017,13 +1023,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" t="n">
         <v>1.0</v>
@@ -1031,10 +1037,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
         <v>72</v>
@@ -1045,10 +1051,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
         <v>73</v>
@@ -1059,10 +1065,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
         <v>74</v>
@@ -1073,10 +1079,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
         <v>75</v>
@@ -1087,10 +1093,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
         <v>76</v>
@@ -1101,66 +1107,66 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
         <v>77</v>
       </c>
-      <c r="B54" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" t="s">
-        <v>79</v>
-      </c>
       <c r="D54" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D56" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
         <v>83</v>
       </c>
       <c r="D57" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
         <v>84</v>
@@ -1171,10 +1177,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
         <v>85</v>
@@ -1185,10 +1191,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
         <v>86</v>
@@ -1199,10 +1205,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
         <v>87</v>
@@ -1213,13 +1219,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" t="s">
         <v>88</v>
-      </c>
-      <c r="B62" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" t="s">
-        <v>89</v>
       </c>
       <c r="D62" t="n">
         <v>1.0</v>
@@ -1227,13 +1233,13 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D63" t="n">
         <v>1.0</v>
@@ -1244,10 +1250,10 @@
         <v>90</v>
       </c>
       <c r="B64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" t="s">
         <v>91</v>
-      </c>
-      <c r="C64" t="s">
-        <v>93</v>
       </c>
       <c r="D64" t="n">
         <v>1.0</v>
@@ -1255,10 +1261,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C65" t="s">
         <v>94</v>
@@ -1269,15 +1275,43 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C66" t="s">
         <v>95</v>
       </c>
       <c r="D66" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>92</v>
+      </c>
+      <c r="B67" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" t="s">
+        <v>96</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" t="n">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>